<commit_message>
changes due to feedback
</commit_message>
<xml_diff>
--- a/Assignments/Implementation_Plan/Implementations plan.xlsx
+++ b/Assignments/Implementation_Plan/Implementations plan.xlsx
@@ -11,107 +11,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+  <si>
+    <t>Importance - 1 least, 5 most</t>
+  </si>
+  <si>
+    <t>use cases</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Move player</t>
+  </si>
+  <si>
+    <t>Start game</t>
+  </si>
+  <si>
+    <t>Fetch twitter feed</t>
+  </si>
+  <si>
+    <t>Enter new room</t>
+  </si>
+  <si>
+    <t>Start fight</t>
+  </si>
+  <si>
+    <t>Item description</t>
+  </si>
+  <si>
+    <t>Combine items</t>
+  </si>
+  <si>
+    <t>Use item</t>
+  </si>
+  <si>
+    <t>Pick up item</t>
+  </si>
+  <si>
+    <t>Drop item</t>
+  </si>
+  <si>
+    <t>Give item</t>
+  </si>
+  <si>
+    <t>Use item on character</t>
+  </si>
+  <si>
+    <t>Open/Close inventory</t>
+  </si>
+  <si>
+    <t>Player to character interaction</t>
+  </si>
+  <si>
+    <t>Start menu</t>
+  </si>
+  <si>
+    <t>Start new single player game</t>
+  </si>
+  <si>
+    <t>Start multiplayer game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create character </t>
+  </si>
+  <si>
+    <t>Player chat</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Prio 5</t>
+  </si>
+  <si>
+    <t>Prio 4</t>
+  </si>
+  <si>
+    <t>Prio 3</t>
+  </si>
+  <si>
+    <t>Prio 2</t>
+  </si>
+  <si>
+    <t>Prio 1</t>
+  </si>
   <si>
     <t xml:space="preserve">Total points 240 per iteration </t>
   </si>
   <si>
-    <t>importance</t>
-  </si>
-  <si>
-    <t>use cases</t>
-  </si>
-  <si>
-    <t>Max Points</t>
-  </si>
-  <si>
-    <t>Min Points</t>
-  </si>
-  <si>
-    <t>Average Points</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Move Player*</t>
-  </si>
-  <si>
-    <t>Start Game*</t>
-  </si>
-  <si>
-    <t>Fetch Twitter Feed</t>
-  </si>
-  <si>
-    <t>Enter New Room</t>
-  </si>
-  <si>
-    <t>Start Fight</t>
-  </si>
-  <si>
-    <t>Item Description</t>
-  </si>
-  <si>
-    <t>Combine Items</t>
-  </si>
-  <si>
-    <t>Use Item</t>
-  </si>
-  <si>
-    <t>Pick up Item</t>
-  </si>
-  <si>
-    <t>Drop Item</t>
-  </si>
-  <si>
-    <t>Give Item</t>
-  </si>
-  <si>
-    <t>No Estimate</t>
-  </si>
-  <si>
-    <t>Use Item On Character</t>
-  </si>
-  <si>
-    <t>Open/Close Inventory</t>
-  </si>
-  <si>
-    <t>Player interaction</t>
-  </si>
-  <si>
-    <t>Start Menu*</t>
-  </si>
-  <si>
-    <t>Start Singleplayer*</t>
-  </si>
-  <si>
-    <t>Start Multiplayer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create character </t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Prio 5</t>
-  </si>
-  <si>
-    <t>Prio 4</t>
-  </si>
-  <si>
-    <t>Prio 3</t>
-  </si>
-  <si>
-    <t>Prio 2</t>
-  </si>
-  <si>
-    <t>Prio 1</t>
-  </si>
-  <si>
     <t>Iteration 1</t>
   </si>
   <si>
@@ -130,19 +121,7 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Start Menu</t>
-  </si>
-  <si>
-    <t>Start Singleplayer</t>
-  </si>
-  <si>
-    <t>Start Game</t>
-  </si>
-  <si>
-    <t>Move Player</t>
-  </si>
-  <si>
-    <t>Gather Twitter Feed</t>
+    <t>Start single player</t>
   </si>
   <si>
     <t>Create character</t>
@@ -151,27 +130,12 @@
     <t>Total points</t>
   </si>
   <si>
-    <t>iteration 2</t>
+    <t>Iteration 2</t>
   </si>
   <si>
     <t xml:space="preserve">Open/Close inventory </t>
   </si>
   <si>
-    <t>Pick up item</t>
-  </si>
-  <si>
-    <t>Drop item</t>
-  </si>
-  <si>
-    <t>Use item</t>
-  </si>
-  <si>
-    <t>Start fight</t>
-  </si>
-  <si>
-    <t>Combine items</t>
-  </si>
-  <si>
     <t>Iteration 3</t>
   </si>
   <si>
@@ -179,12 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">Use item on character </t>
-  </si>
-  <si>
-    <t>Give item</t>
-  </si>
-  <si>
-    <t>Item description</t>
   </si>
   <si>
     <t>Start multiplayer</t>
@@ -229,7 +187,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -237,9 +204,6 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -262,37 +226,32 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.86"/>
-    <col customWidth="1" min="2" max="2" width="26.14"/>
+    <col customWidth="1" min="1" max="1" width="25.86"/>
+    <col customWidth="1" min="2" max="2" width="30.0"/>
     <col customWidth="1" min="3" max="3" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
@@ -302,322 +261,249 @@
         <v>5.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>4.0</v>
       </c>
-      <c r="D5" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>4.0</v>
       </c>
-      <c r="D6" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1">
         <v>5.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>36.0</v>
       </c>
-      <c r="D7" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>24.0</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1">
         <v>5.0</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>36.0</v>
       </c>
-      <c r="D8" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>24.0</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="1">
         <v>3.0</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>16.0</v>
       </c>
-      <c r="D9" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10.0</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1">
         <v>1.0</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>6.0</v>
       </c>
-      <c r="D10" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1">
         <v>2.0</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>36.0</v>
       </c>
-      <c r="D11" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>24.0</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>3.0</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>12.0</v>
       </c>
-      <c r="D12" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8.0</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1">
         <v>3.0</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>12.0</v>
       </c>
-      <c r="D13" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6.0</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>3.0</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>18.0</v>
       </c>
-      <c r="D14" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>12.0</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1">
         <v>1.0</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>72.0</v>
       </c>
-      <c r="D15" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16">
       <c r="A16" s="1">
         <v>1.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>72.0</v>
       </c>
-      <c r="D16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17">
       <c r="A17" s="1">
         <v>4.0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>20</v>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>36.0</v>
       </c>
-      <c r="D17" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>24.0</v>
-      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1">
         <v>1.0</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>72.0</v>
       </c>
-      <c r="D18" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19">
       <c r="A19" s="1">
         <v>5.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>12.0</v>
       </c>
-      <c r="D19" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>8.0</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1">
         <v>5.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>12.0</v>
       </c>
-      <c r="D20" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>8.0</v>
-      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1">
         <v>1.0</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C21" s="1">
         <v>72.0</v>
       </c>
-      <c r="D21" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22">
       <c r="A22" s="1">
         <v>5.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1">
         <v>6.0</v>
       </c>
-      <c r="D22" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>4.0</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1">
+        <v>36.0</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
@@ -628,29 +514,22 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(C5:C23)</f>
+        <v>570</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" ref="C26:E26" si="1">sum(C5:C25)</f>
-        <v>534</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>308</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -660,101 +539,90 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="A28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="6">
+        <f>SUM(C5:C8,C19:C20,C22)</f>
+        <v>110</v>
+      </c>
+      <c r="D28" s="6"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1">
-        <v>110.0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>42.0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>76.0</v>
-      </c>
+      <c r="A29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="6">
+        <f>SUM(C17,)</f>
+        <v>36</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>24.0</v>
-      </c>
+      <c r="A30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="6">
+        <f>SUM(C9,C12:C14,)</f>
+        <v>58</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="1">
-        <v>58.0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>36.0</v>
-      </c>
+      <c r="A31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="6">
+        <f>SUM(C11,)</f>
+        <v>36</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>36.0</v>
-      </c>
-      <c r="D32">
-        <v>12.0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>24.0</v>
-      </c>
+        <f>SUM(C10, C15, C16, C18, C21, C23)</f>
+        <v>330</v>
+      </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="1">
-        <v>294.0</v>
-      </c>
-      <c r="D33">
-        <v>6.0</v>
-      </c>
-      <c r="E33" s="1">
-        <v>148.0</v>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="F36" s="1"/>
     </row>
     <row r="37">
       <c r="A37" s="1"/>
@@ -764,8 +632,8 @@
       <c r="A38" s="1">
         <v>5.0</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>39</v>
+      <c r="B38" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C38" s="1">
         <v>12.0</v>
@@ -781,8 +649,8 @@
       <c r="A39" s="1">
         <v>5.0</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>40</v>
+      <c r="B39" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C39" s="1">
         <v>12.0</v>
@@ -798,8 +666,8 @@
       <c r="A40" s="1">
         <v>5.0</v>
       </c>
-      <c r="B40" t="s">
-        <v>41</v>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C40" s="1">
         <v>4.0</v>
@@ -816,7 +684,7 @@
         <v>4.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1">
         <v>4.0</v>
@@ -833,7 +701,7 @@
         <v>5.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1">
         <v>36.0</v>
@@ -850,7 +718,7 @@
         <v>5.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1">
         <v>36.0</v>
@@ -867,7 +735,7 @@
         <v>5.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1">
         <v>6.0</v>
@@ -881,16 +749,19 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C45" s="1">
-        <v>110.0</v>
+        <f t="shared" ref="C45:E45" si="1">SUM(C38:C44)</f>
+        <v>110</v>
       </c>
       <c r="D45" s="1">
-        <v>42.0</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="E45" s="1">
-        <v>76.0</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
     </row>
     <row r="46">
@@ -901,7 +772,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -909,19 +780,19 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="50">
@@ -929,7 +800,7 @@
         <v>4.0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C50" s="1">
         <v>36.0</v>
@@ -946,7 +817,7 @@
         <v>3.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C51" s="1">
         <v>12.0</v>
@@ -963,7 +834,7 @@
         <v>3.0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C52" s="1">
         <v>18.0</v>
@@ -980,7 +851,7 @@
         <v>3.0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C53" s="1">
         <v>12.0</v>
@@ -997,7 +868,7 @@
         <v>3.0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
         <v>16.0</v>
@@ -1014,7 +885,7 @@
         <v>2.0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C55" s="1">
         <v>36.0</v>
@@ -1028,38 +899,41 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C56" s="1">
-        <v>120.0</v>
+        <f t="shared" ref="C56:E56" si="2">SUM(C50:C55)</f>
+        <v>130</v>
       </c>
       <c r="D56" s="1">
-        <v>40.0</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="E56" s="1">
-        <v>84.0</v>
+        <f t="shared" si="2"/>
+        <v>84</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="60">
@@ -1067,7 +941,7 @@
         <v>1.0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C60" s="1">
         <v>72.0</v>
@@ -1084,13 +958,13 @@
         <v>1.0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C61" s="1">
         <v>72.0</v>
       </c>
       <c r="D61" s="1">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="E61" s="1">
         <v>36.0</v>
@@ -1101,13 +975,13 @@
         <v>1.0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="C62" s="1">
         <v>72.0</v>
       </c>
       <c r="D62" s="1">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="E62" s="1">
         <v>36.0</v>
@@ -1118,7 +992,7 @@
         <v>1.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C63" s="1">
         <v>6.0</v>
@@ -1135,13 +1009,13 @@
         <v>1.0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C64" s="1">
         <v>72.0</v>
       </c>
       <c r="D64" s="1">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="E64" s="1">
         <v>36.0</v>
@@ -1149,16 +1023,19 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C65" s="1">
-        <v>294.0</v>
+        <f t="shared" ref="C65:E65" si="3">SUM(C60:C64)</f>
+        <v>294</v>
       </c>
       <c r="D65" s="1">
-        <v>17.0</v>
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
       <c r="E65" s="1">
-        <v>148.0</v>
+        <f t="shared" si="3"/>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>